<commit_message>
ajuste en el calculo de los lookahead y exportacion de estados a excel
</commit_message>
<xml_diff>
--- a/Tablas a mano.xlsx
+++ b/Tablas a mano.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\1  Universidad\Compiladores\ProyectoCompiladores\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217BC4C-FF6A-41D6-9B3C-F844F4F2DD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE0F357-4FF4-4127-BA85-7A7AD842814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{7615DC9F-7357-481C-A74A-B695FEE1BA0B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="135">
   <si>
     <t>Simbolo</t>
   </si>
@@ -445,73 +445,7 @@
     <t>$</t>
   </si>
   <si>
-    <t>'PROGRAM'</t>
-  </si>
-  <si>
-    <t>&lt;block&gt;</t>
-  </si>
-  <si>
-    <t>&lt;declarations&gt;</t>
-  </si>
-  <si>
-    <t>&lt;var_declaration&gt;</t>
-  </si>
-  <si>
-    <t>&lt;procedure_declaration&gt;</t>
-  </si>
-  <si>
-    <t>'VAR'</t>
-  </si>
-  <si>
-    <t>'PROCEDURE'</t>
-  </si>
-  <si>
-    <t>Siguiente</t>
-  </si>
-  <si>
     <t>.'PROGRAM' identifier ';' &lt;block&gt; '.'</t>
-  </si>
-  <si>
-    <t>PROGRAM' identifier .';' &lt;block&gt; '.'</t>
-  </si>
-  <si>
-    <t>PROGRAM' identifier ';' .&lt;block&gt; '.'</t>
-  </si>
-  <si>
-    <t>.&lt;declarations&gt; &lt;compound_statement&gt;</t>
-  </si>
-  <si>
-    <t>.&lt;var_declaration&gt; &lt;declarations&gt;</t>
-  </si>
-  <si>
-    <t>.&lt;procedure_declaration&gt; &lt;declarations&gt;</t>
-  </si>
-  <si>
-    <t>.e</t>
-  </si>
-  <si>
-    <t>.'VAR' identifier ':' &lt;type&gt; ';' &lt;var_declaration&gt;</t>
-  </si>
-  <si>
-    <t>.'PROCEDURE' identifier '(' &lt;parameter_list&gt; ')' ';' &lt;block&gt; ';'</t>
-  </si>
-  <si>
-    <t>'PROGRAM' .identifier ';' &lt;block&gt; '.'</t>
-  </si>
-  <si>
-    <t>&lt;declarations&gt; .&lt;compound_statement&gt;</t>
-  </si>
-  <si>
-    <t>';'</t>
-  </si>
-  <si>
-    <t>'PROGRAM' .identifier ';' &lt;block&gt; .'.'</t>
-  </si>
-  <si>
-    <t>.'BEGIN' &lt;statement_list&gt; 'END'</t>
-  </si>
-  <si>
-    <t>&lt;var_declaration&gt; .&lt;declarations&gt;</t>
   </si>
 </sst>
 </file>
@@ -572,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -839,7 +773,24 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -852,10 +803,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -864,9 +815,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -879,112 +828,8 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -996,7 +841,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1055,121 +900,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2199,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEDABF6-F07B-4486-923B-94213FC45D57}">
-  <dimension ref="A1:L70"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,14 +1993,14 @@
     <col min="5" max="5" width="21.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.85546875" style="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" style="29" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="26" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" style="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="20"/>
     <col min="11" max="11" width="23.28515625" style="20" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>129</v>
       </c>
@@ -2231,757 +2010,413 @@
       <c r="C1" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="H1" s="46"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="23">
         <v>0</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27">
+      <c r="F2" s="24"/>
+      <c r="G2" s="32">
         <v>0</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="J2" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>2</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="J3" s="20">
-        <v>5</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="L3" s="20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="35"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20">
         <v>3</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="J4" s="20">
-        <v>5</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="L4" s="20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>4</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="46"/>
-      <c r="J5" s="20">
-        <v>5</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>5</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E6" s="25">
-        <f>E2+1</f>
-        <v>1</v>
-      </c>
-      <c r="F6" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="G6" s="27">
-        <v>0</v>
-      </c>
-      <c r="H6" s="46"/>
-      <c r="J6" s="20">
-        <v>5</v>
-      </c>
-      <c r="K6" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="L6" s="20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="36"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H7" s="46"/>
-      <c r="J7" s="20">
-        <v>5</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="L7" s="20">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="36"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E8" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="H8" s="46"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="36"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="46"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="36"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>9</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="25">
-        <f>E6+1</f>
-        <v>2</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="27">
-        <v>1</v>
-      </c>
-      <c r="H10" s="46"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="36"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="46"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H11" s="36"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>11</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>143</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="46"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="36"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>12</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H13" s="46"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="36"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>13</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="25">
-        <f>E10+1</f>
-        <v>3</v>
-      </c>
-      <c r="F14" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="G14" s="27">
-        <f>E10</f>
-        <v>2</v>
-      </c>
-      <c r="H14" s="46"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="36"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>14</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H15" s="46"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H15" s="36"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="46"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="20">
         <v>16</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="42" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="43" t="s">
-        <v>145</v>
-      </c>
-      <c r="G17" s="44" t="str">
-        <f>G16</f>
-        <v>$</v>
-      </c>
-      <c r="H17" s="46"/>
+      <c r="H17" s="36"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="20">
         <v>17</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="G18" s="40" t="str">
-        <f t="shared" ref="G18:G23" si="0">G17</f>
-        <v>$</v>
-      </c>
-      <c r="H18" s="46"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="G19" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>$</v>
-      </c>
-      <c r="H19" s="50"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>19</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="E20" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="G20" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>$</v>
-      </c>
-      <c r="H20" s="50"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>20</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="G21" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>$</v>
-      </c>
-      <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>21</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>148</v>
-      </c>
-      <c r="G22" s="40" t="str">
-        <f t="shared" si="0"/>
-        <v>$</v>
-      </c>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>22</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>150</v>
-      </c>
-      <c r="G23" s="35" t="str">
-        <f>G22</f>
-        <v>$</v>
-      </c>
-      <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>23</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F24" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>24</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E25" s="25">
-        <f>E14+1</f>
-        <v>4</v>
-      </c>
-      <c r="F25" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G25" s="27">
-        <f>E14</f>
-        <v>3</v>
-      </c>
-      <c r="H25" s="50"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>25</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H26" s="50"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>26</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="H27" s="50"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>27</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E28" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F28" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G28" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H28" s="51"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
         <v>28</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="25">
-        <f>E25+1</f>
-        <v>5</v>
-      </c>
-      <c r="F29" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="G29" s="27">
-        <f>E$14</f>
-        <v>3</v>
-      </c>
-      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>29</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F30" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G30" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H30" s="51"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="20">
         <v>30</v>
       </c>
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="E31" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="48" t="s">
-        <v>152</v>
-      </c>
-      <c r="G31" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="H31" s="58"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="20">
         <v>31</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E32" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="G32" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="H32" s="50"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>32</v>
       </c>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="30" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="G33" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="H33" s="51"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20">
         <v>33</v>
       </c>
@@ -2991,20 +2426,8 @@
       <c r="C34" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="25">
-        <f>E29+1</f>
-        <v>6</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="G34" s="27">
-        <f>E$14</f>
-        <v>3</v>
-      </c>
-      <c r="H34" s="51"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20">
         <v>34</v>
       </c>
@@ -3014,18 +2437,8 @@
       <c r="C35" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="22" t="s">
-        <v>123</v>
-      </c>
-      <c r="F35" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="G35" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="H35" s="51"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>35</v>
       </c>
@@ -3035,18 +2448,8 @@
       <c r="C36" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>133</v>
-      </c>
-      <c r="H36" s="51"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20">
         <v>36</v>
       </c>
@@ -3056,18 +2459,8 @@
       <c r="C37" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="E37" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F37" s="51" t="s">
-        <v>146</v>
-      </c>
-      <c r="G37" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H37" s="51"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="20">
         <v>37</v>
       </c>
@@ -3077,18 +2470,8 @@
       <c r="C38" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E38" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="G38" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H38" s="51"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20">
         <v>38</v>
       </c>
@@ -3098,18 +2481,8 @@
       <c r="C39" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F39" s="51" t="s">
-        <v>148</v>
-      </c>
-      <c r="G39" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H39" s="51"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="20">
         <v>39</v>
       </c>
@@ -3119,18 +2492,8 @@
       <c r="C40" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E40" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="G40" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H40" s="51"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>40</v>
       </c>
@@ -3140,18 +2503,8 @@
       <c r="C41" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="E41" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="55" t="s">
-        <v>148</v>
-      </c>
-      <c r="G41" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H41" s="51"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>41</v>
       </c>
@@ -3161,18 +2514,8 @@
       <c r="C42" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E42" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="G42" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="H42" s="51"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>42</v>
       </c>
@@ -3182,12 +2525,8 @@
       <c r="C43" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E43" s="56"/>
-      <c r="F43" s="56"/>
-      <c r="G43" s="56"/>
-      <c r="H43" s="51"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20">
         <v>43</v>
       </c>
@@ -3197,12 +2536,8 @@
       <c r="C44" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="56"/>
-      <c r="G44" s="56"/>
-      <c r="H44" s="51"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20">
         <v>44</v>
       </c>
@@ -3212,12 +2547,8 @@
       <c r="C45" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="51"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20">
         <v>45</v>
       </c>
@@ -3227,12 +2558,8 @@
       <c r="C46" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="51"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="20">
         <v>46</v>
       </c>
@@ -3242,12 +2569,8 @@
       <c r="C47" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="56"/>
-      <c r="H47" s="51"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="20">
         <v>47</v>
       </c>
@@ -3257,12 +2580,8 @@
       <c r="C48" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="56"/>
-      <c r="H48" s="51"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="20">
         <v>48</v>
       </c>
@@ -3272,12 +2591,8 @@
       <c r="C49" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="51"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="20">
         <v>49</v>
       </c>
@@ -3287,12 +2602,9 @@
       <c r="C50" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="56"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="51"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F50" s="25"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="20">
         <v>50</v>
       </c>
@@ -3302,12 +2614,8 @@
       <c r="C51" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="51"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="20">
         <v>51</v>
       </c>
@@ -3317,12 +2625,9 @@
       <c r="C52" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="51"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F52" s="25"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="20">
         <v>52</v>
       </c>
@@ -3332,12 +2637,8 @@
       <c r="C53" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="51"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="20">
         <v>53</v>
       </c>
@@ -3347,12 +2648,8 @@
       <c r="C54" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="51"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="20">
         <v>54</v>
       </c>
@@ -3362,12 +2659,9 @@
       <c r="C55" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E55" s="56"/>
-      <c r="F55" s="57"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="51"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F55" s="25"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="20">
         <v>55</v>
       </c>
@@ -3377,12 +2671,8 @@
       <c r="C56" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="51"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="20">
         <v>56</v>
       </c>
@@ -3392,12 +2682,9 @@
       <c r="C57" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E57" s="56"/>
-      <c r="F57" s="57"/>
-      <c r="G57" s="56"/>
-      <c r="H57" s="51"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F57" s="25"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="20">
         <v>57</v>
       </c>
@@ -3407,12 +2694,8 @@
       <c r="C58" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="E58" s="56"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="51"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="20">
         <v>58</v>
       </c>
@@ -3422,12 +2705,9 @@
       <c r="C59" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E59" s="56"/>
-      <c r="F59" s="57"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="51"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F59" s="25"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="20">
         <v>59</v>
       </c>
@@ -3437,12 +2717,8 @@
       <c r="C60" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E60" s="56"/>
-      <c r="F60" s="56"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="51"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="20">
         <v>60</v>
       </c>
@@ -3452,12 +2728,9 @@
       <c r="C61" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E61" s="56"/>
-      <c r="F61" s="57"/>
-      <c r="G61" s="56"/>
-      <c r="H61" s="51"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F61" s="25"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="20">
         <v>61</v>
       </c>
@@ -3467,12 +2740,8 @@
       <c r="C62" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="51"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="20">
         <v>62</v>
       </c>
@@ -3482,12 +2751,9 @@
       <c r="C63" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E63" s="56"/>
-      <c r="F63" s="57"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="51"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F63" s="25"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="20">
         <v>63</v>
       </c>
@@ -3497,46 +2763,12 @@
       <c r="C64" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="51"/>
-    </row>
-    <row r="65" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E65" s="56"/>
-      <c r="F65" s="57"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="51"/>
-    </row>
-    <row r="66" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="51"/>
-    </row>
-    <row r="67" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="51"/>
-    </row>
-    <row r="68" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E68" s="56"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="51"/>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="51"/>
-    </row>
-    <row r="70" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="51"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F65" s="25"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F68" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C65" xr:uid="{3CEDABF6-F07B-4486-923B-94213FC45D57}">

</xml_diff>